<commit_message>
correction: when modifying a material, in case the new unit measures a magnitude other than the current unit, then the current unit is kept unchanged.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/acquirable_material_modify_test_cases.xlsx
+++ b/soberano/test_cases/acquirable_material_modify_test_cases.xlsx
@@ -175,31 +175,31 @@
     <t xml:space="preserve">mm93</t>
   </si>
   <si>
-    <t xml:space="preserve">check mm1 data is correctly shown in details panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check mm2 data is correctly shown in details panel</t>
+    <t xml:space="preserve">check mm1 data is correctly shown in details panel. Unit keeps unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check mm2 data is correctly shown in details panel. Unit keeps unchanged.</t>
   </si>
   <si>
     <t xml:space="preserve">check mm3 data is correctly shown in details panel</t>
   </si>
   <si>
-    <t xml:space="preserve">check mm4 data is correctly shown in details panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check mm5 data is correctly shown in details panel</t>
+    <t xml:space="preserve">check mm4 data is correctly shown in details panel. Unit keeps unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check mm5 data is correctly shown in details panel. Unit keeps unchanged.</t>
   </si>
   <si>
     <t xml:space="preserve">check mm6 data is correctly shown in details panel</t>
   </si>
   <si>
-    <t xml:space="preserve">check mm7 data is correctly shown in details panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check mm8 data is correctly shown in details panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check mm9 data is correctly shown in details panel</t>
+    <t xml:space="preserve">check mm7 data is correctly shown in details panel. Unit keeps unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check mm8 data is correctly shown in details panel. Unit keeps unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check mm9 data is correctly shown in details panel. Unit keeps unchanged.</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -245,11 +245,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Monospace"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -327,10 +322,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,8 +344,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -617,7 +608,7 @@
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="2" t="n">

</xml_diff>

<commit_message>
from spi form, prevent to move items when origin and destination warehouse are the same.
customer printer profiles added.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/acquirable_material_modify_test_cases.xlsx
+++ b/soberano/test_cases/acquirable_material_modify_test_cases.xlsx
@@ -49,21 +49,21 @@
     <t xml:space="preserve">mmaterial1</t>
   </si>
   <si>
+    <t xml:space="preserve">piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User2 is NOT allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmaterial2</t>
+  </si>
+  <si>
     <t xml:space="preserve">kilogram</t>
   </si>
   <si>
-    <t xml:space="preserve">User2 is NOT allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmaterial2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">piece</t>
-  </si>
-  <si>
     <t xml:space="preserve">User3 is allowed to modify acquirable material</t>
   </si>
   <si>
@@ -91,49 +91,49 @@
     <t xml:space="preserve">mmaterial4</t>
   </si>
   <si>
+    <t xml:space="preserve">milligram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User7 is allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User8 is NOT allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmaterial5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User9 is allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User10 is NOT allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmaterial6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User11 is allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User12 is NOT allowed to modify acquirable material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmaterial7</t>
+  </si>
+  <si>
     <t xml:space="preserve">milliliter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User7 is allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User8 is NOT allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmaterial5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User9 is allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User10 is NOT allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmaterial6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">milligram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User11 is allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User12 is NOT allowed to modify acquirable material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmaterial7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pound</t>
   </si>
   <si>
     <t xml:space="preserve">User13 is allowed to modify acquirable material</t>
@@ -344,8 +344,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,7 +549,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>4</v>
@@ -560,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -569,7 +569,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>4</v>
@@ -580,16 +580,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>400.00004</v>
@@ -603,13 +603,13 @@
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>400.00004</v>
@@ -669,7 +669,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>3</v>
@@ -689,7 +689,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>3</v>
@@ -709,7 +709,7 @@
         <v>45</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>100.00001</v>
@@ -729,7 +729,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>100.00001</v>
@@ -749,7 +749,7 @@
         <v>48</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>12800.00128</v>
@@ -769,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>12800.00128</v>

</xml_diff>